<commit_message>
Therewaserror when user has one booking.This fixed
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -424,10 +424,10 @@
         <v>aksoy</v>
       </c>
       <c r="C2" t="str">
-        <v>01.08.2022</v>
+        <v>08.08.2022</v>
       </c>
       <c r="D2" t="str">
-        <v>Desk B35</v>
+        <v>Desk B86</v>
       </c>
     </row>
     <row r="3">
@@ -438,16 +438,72 @@
         <v>aksoy</v>
       </c>
       <c r="C3" t="str">
-        <v>04.08.2022</v>
+        <v>01.08.2022</v>
       </c>
       <c r="D3" t="str">
         <v>Desk B35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve">Dilara </v>
+      </c>
+      <c r="B4" t="str">
+        <v>aksoy</v>
+      </c>
+      <c r="C4" t="str">
+        <v>04.08.2022</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Desk B35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v xml:space="preserve">Dilara </v>
+      </c>
+      <c r="B5" t="str">
+        <v>aksoy</v>
+      </c>
+      <c r="C5" t="str">
+        <v>09.08.2022</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Desk B71</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v xml:space="preserve">Dilara </v>
+      </c>
+      <c r="B6" t="str">
+        <v>aksoy</v>
+      </c>
+      <c r="C6" t="str">
+        <v>10.08.2022</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Desk B40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">Dilara </v>
+      </c>
+      <c r="B7" t="str">
+        <v>aksoy</v>
+      </c>
+      <c r="C7" t="str">
+        <v>11.08.2022</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Desk B69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
İcon and popup css changed, server improved
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -500,10 +500,24 @@
         <v>Desk B69</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">Dilara </v>
+      </c>
+      <c r="B8" t="str">
+        <v>aksoy</v>
+      </c>
+      <c r="C8" t="str">
+        <v>08.08.2022</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Desk 046</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added a warning to popup
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -424,100 +424,16 @@
         <v>aksoy</v>
       </c>
       <c r="C2" t="str">
-        <v>08.08.2022</v>
+        <v>09.08.2022</v>
       </c>
       <c r="D2" t="str">
-        <v>Desk B86</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v xml:space="preserve">Dilara </v>
-      </c>
-      <c r="B3" t="str">
-        <v>aksoy</v>
-      </c>
-      <c r="C3" t="str">
-        <v>01.08.2022</v>
-      </c>
-      <c r="D3" t="str">
         <v>Desk B35</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v xml:space="preserve">Dilara </v>
-      </c>
-      <c r="B4" t="str">
-        <v>aksoy</v>
-      </c>
-      <c r="C4" t="str">
-        <v>04.08.2022</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Desk B35</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v xml:space="preserve">Dilara </v>
-      </c>
-      <c r="B5" t="str">
-        <v>aksoy</v>
-      </c>
-      <c r="C5" t="str">
-        <v>09.08.2022</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Desk B71</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v xml:space="preserve">Dilara </v>
-      </c>
-      <c r="B6" t="str">
-        <v>aksoy</v>
-      </c>
-      <c r="C6" t="str">
-        <v>10.08.2022</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Desk B40</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve">Dilara </v>
-      </c>
-      <c r="B7" t="str">
-        <v>aksoy</v>
-      </c>
-      <c r="C7" t="str">
-        <v>11.08.2022</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Desk B69</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve">Dilara </v>
-      </c>
-      <c r="B8" t="str">
-        <v>aksoy</v>
-      </c>
-      <c r="C8" t="str">
-        <v>08.08.2022</v>
-      </c>
-      <c r="D8" t="str">
-        <v>Desk 046</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>